<commit_message>
updated scripts with browserstack integration
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Solutions/ccs-enterprise-automation-ui-project/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01146C36-CF4A-2948-9FAB-FB6ED60A513D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{FF93901F-1912-784D-BF8D-A5BF54E1AEF7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="2020" windowWidth="26200" windowHeight="10880" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" tabRatio="752" windowHeight="10880" windowWidth="26200" xWindow="1760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2020"/>
   </bookViews>
   <sheets>
-    <sheet name="Keywords" sheetId="11" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="4" r:id="rId2"/>
-    <sheet name="TC001_SignIn" sheetId="3" r:id="rId3"/>
-    <sheet name="TC002_SignUp" sheetId="10" r:id="rId4"/>
+    <sheet name="Keywords" r:id="rId1" sheetId="11"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="4"/>
+    <sheet name="TC001_SignIn" r:id="rId3" sheetId="3"/>
+    <sheet name="TC002_Login" r:id="rId4" sheetId="10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>TS_02</t>
   </si>
@@ -64,18 +64,9 @@
     <t>To verify that user is able to sign in</t>
   </si>
   <si>
-    <t>TC002_SignUp</t>
-  </si>
-  <si>
     <t>To verify that user is able to sign up</t>
   </si>
   <si>
-    <t>Highlight message in backet</t>
-  </si>
-  <si>
-    <t>Click on basket button</t>
-  </si>
-  <si>
     <t>TS_01</t>
   </si>
   <si>
@@ -139,12 +130,6 @@
     <t>SwitchToFrame</t>
   </si>
   <si>
-    <t>btn_basket</t>
-  </si>
-  <si>
-    <t>elm_message</t>
-  </si>
-  <si>
     <t>TS_03</t>
   </si>
   <si>
@@ -176,15 +161,6 @@
   </si>
   <si>
     <t>EnterSavedValue</t>
-  </si>
-  <si>
-    <t>Save message text on cart page</t>
-  </si>
-  <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>Verify text</t>
   </si>
   <si>
     <t>VerifyElemDisabled</t>
@@ -366,25 +342,59 @@
     <t>To clear value from a text box</t>
   </si>
   <si>
-    <t>To save element text to runtime session data manager. The key will be element name.</t>
-  </si>
-  <si>
-    <t>To save a value to runtime. Pass the key in 'selector' column, and value in 'data' column</t>
-  </si>
-  <si>
-    <t>To verify element text with saved session data. Pass the 'element' as selector and expected 'key' as data.</t>
-  </si>
-  <si>
-    <t>Enter with saved value from session data. Pass the expected key as 'data'</t>
-  </si>
-  <si>
-    <t>To check if element is disabled.</t>
+    <t>TS_04</t>
+  </si>
+  <si>
+    <t>TS_05</t>
+  </si>
+  <si>
+    <t>Wait for email field</t>
+  </si>
+  <si>
+    <t>txt_email</t>
+  </si>
+  <si>
+    <t>pcc.esourcingtest13@yopmail.com</t>
+  </si>
+  <si>
+    <t>Test_12345</t>
+  </si>
+  <si>
+    <t>txt_password</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>Click on sign in button</t>
+  </si>
+  <si>
+    <t>btn_signin</t>
+  </si>
+  <si>
+    <t>Wait for dashboard title</t>
+  </si>
+  <si>
+    <t>elm_header</t>
+  </si>
+  <si>
+    <t>elm_wrong_header</t>
+  </si>
+  <si>
+    <t>TC002_Login</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,54 +498,54 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -552,10 +562,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -590,7 +600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,7 +652,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,7 +757,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -756,13 +766,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -772,7 +782,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -781,7 +791,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -790,7 +800,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -800,12 +810,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -836,7 +846,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -855,7 +865,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -867,288 +877,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D0990-AD1B-5244-AC3C-8B60408730A0}">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D0990-AD1B-5244-AC3C-8B60408730A0}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="142.5" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="9" width="24.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="13" width="142.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+    <row ht="20" r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row ht="20" r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row ht="20" r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row ht="20" r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row ht="20" r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B5" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row ht="20" r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B6" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row ht="20" r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row ht="40" r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row ht="20" r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row ht="40" r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row ht="40" r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row ht="20" r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row ht="20" r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row ht="20" r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row ht="20" r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row ht="20" r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row ht="20" r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="20" r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row ht="20" r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row ht="20" r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row ht="20" r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row ht="20" r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row ht="20" r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row ht="20" r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row ht="20" r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row ht="20" r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="40" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="40" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="40" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.83203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.1640625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="37.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="81.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="10.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="15.83203125" collapsed="true"/>
+    <col min="5" max="16384" style="3" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1165,7 +1160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row customFormat="1" ht="16" r="2" s="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -1179,12 +1174,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row ht="16" r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1195,32 +1190,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" location="TC001_SignIn!A1" display="TC001_SignIn" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" location="TC002_SignUp!A1" display="TC002_SignUp" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink display="TC001_SignIn" location="TC001_SignIn!A1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="TC002_SignUp" location="TC002_SignUp!A1" ref="A3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53.5" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="70.1640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="40.5" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.1640625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="53.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="70.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="40.5" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1239,17 +1234,17 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,59 +1252,80 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>47</v>
+      <c r="D4" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>52</v>
+      <c r="A5" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D5" s="11"/>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D3" xr:uid="{7D2E6ED1-C190-F443-BEB3-42C39AD6D7EA}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1A82EE43-19D1-E849-B185-86D9C39F7226}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{1A82EE43-19D1-E849-B185-86D9C39F7226}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$29</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C250</xm:sqref>
+          <xm:sqref>C2:C251</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1318,24 +1334,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E711B2E9-84E6-C647-AF41-931D98C86C3E}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E711B2E9-84E6-C647-AF41-931D98C86C3E}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53.5" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="70.1640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.1640625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="53.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="70.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="25.0" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1354,17 +1370,17 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2"/>
+        <v>21</v>
+      </c>
+      <c r="D2" s="11"/>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1372,22 +1388,87 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
+      <c r="D5" s="11"/>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C14" xr:uid="{27B9D99F-DC95-694B-9F80-C667522DFFA4}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C7:C13" type="list" xr:uid="{27B9D99F-DC95-694B-9F80-C667522DFFA4}">
       <formula1>"NavigateTo,ClickOnElement,HighlightElement,HoverOnElement"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D3" xr:uid="{AE03CF7E-8F26-F944-8F5B-6031A1DA6B86}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{AAC0343F-A2F4-6B45-81B5-4B2CFF5875A5}">
+          <x14:formula1>
+            <xm:f>Keywords!$A$2:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update-TC005 on the Spreadsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Automation/Conclave UI/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akin.adebayo1/Documents/GitHub/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{76C0C739-AADB-B348-A59A-74B9C64DD8F3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5968A0-2967-4040-A868-EB11E253F4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="752" windowHeight="15880" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" tabRatio="752" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Keywords" r:id="rId1" sheetId="11"/>
-    <sheet name="TestCases" r:id="rId2" sheetId="4"/>
-    <sheet name="TC001_RegBuyerOrganisation" r:id="rId3" sheetId="20"/>
-    <sheet name="TC002_RegSupplierOrganisation" r:id="rId4" sheetId="21"/>
-    <sheet name="TC001_AddDeleteContact" r:id="rId5" sheetId="16"/>
-    <sheet name="TC002_AddDeleteSite" r:id="rId6" sheetId="17"/>
-    <sheet name="TC003_AddDeleteGroup" r:id="rId7" sheetId="18"/>
-    <sheet name="TC004_ResetPassword" r:id="rId8" sheetId="19"/>
+    <sheet name="Keywords" sheetId="11" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="4" r:id="rId2"/>
+    <sheet name="TC001_RegBuyerOrganisation" sheetId="20" r:id="rId3"/>
+    <sheet name="TC002_RegSupplierOrganisation" sheetId="21" r:id="rId4"/>
+    <sheet name="TC001_AddDeleteContact" sheetId="16" r:id="rId5"/>
+    <sheet name="TC002_AddDeleteSite" sheetId="17" r:id="rId6"/>
+    <sheet name="TC003_AddDeleteGroup" sheetId="18" r:id="rId7"/>
+    <sheet name="TC004_ResetPassword" sheetId="19" r:id="rId8"/>
+    <sheet name="TC005-OrgAdminAddUser" sheetId="22" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="TC001_AddDeleteContact">TestCases!#REF!</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="391">
   <si>
     <t>TS_02</t>
   </si>
@@ -1227,12 +1228,110 @@
   <si>
     <t>To enter random text [Format: Automation+random letters (5) ]</t>
   </si>
+  <si>
+    <t>TC005-OrgAdminAddUser</t>
+  </si>
+  <si>
+    <t>To verify that org Admin can add an Org user</t>
+  </si>
+  <si>
+    <t>auto_snr_supplier@yopmail.com</t>
+  </si>
+  <si>
+    <t>Test12345@</t>
+  </si>
+  <si>
+    <t>Click manage users</t>
+  </si>
+  <si>
+    <t>lnk_manage_user</t>
+  </si>
+  <si>
+    <t>Wait for manage your org user accounts page</t>
+  </si>
+  <si>
+    <t>elm_manageOrgUserAccount_header</t>
+  </si>
+  <si>
+    <t>Click add user</t>
+  </si>
+  <si>
+    <t>elm_addUsers</t>
+  </si>
+  <si>
+    <t>TS-13</t>
+  </si>
+  <si>
+    <t>Wait for Add users page</t>
+  </si>
+  <si>
+    <t>elm_addUser_header</t>
+  </si>
+  <si>
+    <t>Select Add single user radio button</t>
+  </si>
+  <si>
+    <t>elm_addSingleUser</t>
+  </si>
+  <si>
+    <t>Click Continue</t>
+  </si>
+  <si>
+    <t>elm_continueButton</t>
+  </si>
+  <si>
+    <t>Enter First name</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>txt.fName</t>
+  </si>
+  <si>
+    <t>Enter Last name</t>
+  </si>
+  <si>
+    <t>txt.lName</t>
+  </si>
+  <si>
+    <t>Enter email Address</t>
+  </si>
+  <si>
+    <t>RandomEmail</t>
+  </si>
+  <si>
+    <t>@yopmail.com</t>
+  </si>
+  <si>
+    <t>txt.eMail_User_registered</t>
+  </si>
+  <si>
+    <t>Select Org User-Dashboard checkbox</t>
+  </si>
+  <si>
+    <t>chk_Org_user_dashboard_checkbox</t>
+  </si>
+  <si>
+    <t>Click User ID and password</t>
+  </si>
+  <si>
+    <t>elm_userID_password</t>
+  </si>
+  <si>
+    <t>Click Save changes</t>
+  </si>
+  <si>
+    <t>elm_save_Changes</t>
+  </si>
+  <si>
+    <t>elm_email_instruction_sent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1366,78 +1465,78 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="7" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="7" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="10" numFmtId="49" xfId="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1454,10 +1553,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1492,7 +1591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1544,7 +1643,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1649,7 +1748,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1658,13 +1757,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1674,7 +1773,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1683,7 +1782,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1692,7 +1791,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1702,12 +1801,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1738,7 +1837,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1757,7 +1856,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1769,8 +1868,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D0990-AD1B-5244-AC3C-8B60408730A0}">
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D0990-AD1B-5244-AC3C-8B60408730A0}">
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
@@ -1778,11 +1877,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="24.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="7" width="142.5" collapsed="true"/>
+    <col min="1" max="1" width="24.1640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="142.5" style="7" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="20" r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1790,7 +1889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="20" r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1798,7 +1897,7 @@
         <v>44</v>
       </c>
     </row>
-    <row ht="20" r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1806,7 +1905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row ht="20" r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1814,7 +1913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row ht="20" r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1822,7 +1921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row ht="20" r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1830,7 +1929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row ht="20" r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1838,7 +1937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row ht="40" r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1846,7 +1945,7 @@
         <v>49</v>
       </c>
     </row>
-    <row ht="20" r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1854,7 +1953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row ht="40" r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="40" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1862,7 +1961,7 @@
         <v>56</v>
       </c>
     </row>
-    <row ht="40" r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="40" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1870,7 +1969,7 @@
         <v>53</v>
       </c>
     </row>
-    <row ht="20" r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1878,7 +1977,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="20" r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1886,7 +1985,7 @@
         <v>55</v>
       </c>
     </row>
-    <row ht="20" r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1894,7 +1993,7 @@
         <v>57</v>
       </c>
     </row>
-    <row ht="20" r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +2001,7 @@
         <v>58</v>
       </c>
     </row>
-    <row ht="20" r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1910,7 +2009,7 @@
         <v>59</v>
       </c>
     </row>
-    <row ht="20" r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1918,7 +2017,7 @@
         <v>60</v>
       </c>
     </row>
-    <row ht="20" r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1926,7 +2025,7 @@
         <v>61</v>
       </c>
     </row>
-    <row ht="20" r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -1934,7 +2033,7 @@
         <v>62</v>
       </c>
     </row>
-    <row ht="20" r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1942,7 +2041,7 @@
         <v>63</v>
       </c>
     </row>
-    <row ht="20" r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1950,7 +2049,7 @@
         <v>64</v>
       </c>
     </row>
-    <row ht="20" r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -1958,7 +2057,7 @@
         <v>65</v>
       </c>
     </row>
-    <row ht="20" r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
@@ -1966,7 +2065,7 @@
         <v>66</v>
       </c>
     </row>
-    <row ht="20" r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>36</v>
       </c>
@@ -1974,7 +2073,7 @@
         <v>67</v>
       </c>
     </row>
-    <row ht="20" r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -1982,7 +2081,7 @@
         <v>68</v>
       </c>
     </row>
-    <row ht="20" r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -1990,7 +2089,7 @@
         <v>69</v>
       </c>
     </row>
-    <row ht="20" r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>39</v>
       </c>
@@ -1998,7 +2097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row ht="20" r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>40</v>
       </c>
@@ -2006,7 +2105,7 @@
         <v>71</v>
       </c>
     </row>
-    <row ht="20" r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>41</v>
       </c>
@@ -2014,7 +2113,7 @@
         <v>72</v>
       </c>
     </row>
-    <row ht="20" r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -2022,7 +2121,7 @@
         <v>73</v>
       </c>
     </row>
-    <row ht="20" r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
@@ -2030,7 +2129,7 @@
         <v>52</v>
       </c>
     </row>
-    <row ht="20" r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>258</v>
       </c>
@@ -2038,7 +2137,7 @@
         <v>259</v>
       </c>
     </row>
-    <row ht="20" r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>266</v>
       </c>
@@ -2046,7 +2145,7 @@
         <v>357</v>
       </c>
     </row>
-    <row ht="20" r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>315</v>
       </c>
@@ -2055,26 +2154,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="37.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="84.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="10.1640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="15.83203125" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.1640625" collapsed="true"/>
+    <col min="1" max="1" width="37.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="84.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.83203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.1640625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2119,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>169</v>
       </c>
@@ -2173,20 +2272,28 @@
         <v>294</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="TC001_AddDeleteContact" location="TC001_AddDeleteContact!A1" ref="A4" xr:uid="{495083B3-A086-144F-A4CB-0341CFDA339F}"/>
-    <hyperlink display="TC002_AddDeleteSite" location="TC002_AddDeleteSite!A1" ref="A5" xr:uid="{12310066-B5F4-5247-823C-528CB73E0F44}"/>
-    <hyperlink display="TC001_RegisterOrganisation" location="TC001_RegisterOrganisation!A1" ref="A2" xr:uid="{29AF2AF6-6A01-984E-8D48-D603E44F5F2E}"/>
-    <hyperlink display="TC002_RegSupplierOrganisation" location="TC002_RegSupplierOrganisation!A1" ref="A3" xr:uid="{79B13C14-1218-F243-B661-5C545C3D0C79}"/>
+    <hyperlink ref="A4" location="TC001_AddDeleteContact!A1" display="TC001_AddDeleteContact" xr:uid="{495083B3-A086-144F-A4CB-0341CFDA339F}"/>
+    <hyperlink ref="A5" location="TC002_AddDeleteSite!A1" display="TC002_AddDeleteSite" xr:uid="{12310066-B5F4-5247-823C-528CB73E0F44}"/>
+    <hyperlink ref="A2" location="TC001_RegisterOrganisation!A1" display="TC001_RegisterOrganisation" xr:uid="{29AF2AF6-6A01-984E-8D48-D603E44F5F2E}"/>
+    <hyperlink ref="A3" location="TC002_RegSupplierOrganisation!A1" display="TC002_RegSupplierOrganisation" xr:uid="{79B13C14-1218-F243-B661-5C545C3D0C79}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668AFD03-FEF2-3140-AF6D-190EC0470E79}">
-  <dimension ref="A1:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668AFD03-FEF2-3140-AF6D-190EC0470E79}">
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -2194,13 +2301,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="65.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="43.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="2" max="2" width="65.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="21" r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -2217,7 +2324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="21" r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -2232,7 +2339,7 @@
         <v>103</v>
       </c>
     </row>
-    <row ht="21" r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +2354,7 @@
         <v>244</v>
       </c>
     </row>
-    <row ht="21" r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -2262,7 +2369,7 @@
         <v>246</v>
       </c>
     </row>
-    <row ht="21" r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>74</v>
       </c>
@@ -2277,7 +2384,7 @@
         <v>248</v>
       </c>
     </row>
-    <row ht="21" r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>75</v>
       </c>
@@ -2292,7 +2399,7 @@
         <v>250</v>
       </c>
     </row>
-    <row ht="21" r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -2307,7 +2414,7 @@
         <v>252</v>
       </c>
     </row>
-    <row ht="21" r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
@@ -2324,7 +2431,7 @@
         <v>261</v>
       </c>
     </row>
-    <row ht="21" r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -2341,7 +2448,7 @@
         <v>262</v>
       </c>
     </row>
-    <row ht="21" r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -2358,7 +2465,7 @@
         <v>263</v>
       </c>
     </row>
-    <row ht="21" r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>86</v>
       </c>
@@ -2373,7 +2480,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>87</v>
       </c>
@@ -2387,7 +2494,7 @@
         <v>268</v>
       </c>
     </row>
-    <row ht="21" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -2402,7 +2509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -2416,7 +2523,7 @@
         <v>270</v>
       </c>
     </row>
-    <row ht="21" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -2430,7 +2537,7 @@
         <v>270</v>
       </c>
     </row>
-    <row ht="21" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
@@ -2445,7 +2552,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>94</v>
       </c>
@@ -2459,7 +2566,7 @@
         <v>273</v>
       </c>
     </row>
-    <row ht="21" r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
@@ -2473,7 +2580,7 @@
         <v>275</v>
       </c>
     </row>
-    <row ht="21" r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>96</v>
       </c>
@@ -2488,7 +2595,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>97</v>
       </c>
@@ -2502,7 +2609,7 @@
         <v>277</v>
       </c>
     </row>
-    <row ht="21" r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>152</v>
       </c>
@@ -2516,7 +2623,7 @@
         <v>279</v>
       </c>
     </row>
-    <row ht="21" r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>153</v>
       </c>
@@ -2531,7 +2638,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>154</v>
       </c>
@@ -2545,7 +2652,7 @@
         <v>281</v>
       </c>
     </row>
-    <row ht="21" r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>155</v>
       </c>
@@ -2559,7 +2666,7 @@
         <v>283</v>
       </c>
     </row>
-    <row ht="21" r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>162</v>
       </c>
@@ -2576,7 +2683,7 @@
         <v>285</v>
       </c>
     </row>
-    <row ht="21" r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>165</v>
       </c>
@@ -2591,7 +2698,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>166</v>
       </c>
@@ -2605,7 +2712,7 @@
         <v>287</v>
       </c>
     </row>
-    <row ht="21" r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>167</v>
       </c>
@@ -2619,7 +2726,7 @@
         <v>289</v>
       </c>
     </row>
-    <row ht="21" r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>182</v>
       </c>
@@ -2634,7 +2741,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>183</v>
       </c>
@@ -2648,7 +2755,7 @@
         <v>291</v>
       </c>
     </row>
-    <row ht="21" r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>184</v>
       </c>
@@ -2663,7 +2770,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>185</v>
       </c>
@@ -2679,11 +2786,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{673DA5EE-7797-4E4A-9773-9F2C7C77CD06}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{673DA5EE-7797-4E4A-9773-9F2C7C77CD06}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$33</xm:f>
           </x14:formula1>
@@ -2696,8 +2803,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3352E-5FAD-A043-B815-800E1B99D5C6}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3352E-5FAD-A043-B815-800E1B99D5C6}">
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -2705,13 +2812,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="65.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="43.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="2" max="2" width="65.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="21" r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -2728,7 +2835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="21" r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -2743,7 +2850,7 @@
         <v>103</v>
       </c>
     </row>
-    <row ht="21" r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2865,7 @@
         <v>244</v>
       </c>
     </row>
-    <row ht="21" r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -2773,7 +2880,7 @@
         <v>246</v>
       </c>
     </row>
-    <row ht="21" r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>74</v>
       </c>
@@ -2788,7 +2895,7 @@
         <v>248</v>
       </c>
     </row>
-    <row ht="21" r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>75</v>
       </c>
@@ -2803,7 +2910,7 @@
         <v>250</v>
       </c>
     </row>
-    <row ht="21" r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -2818,7 +2925,7 @@
         <v>252</v>
       </c>
     </row>
-    <row ht="21" r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
@@ -2835,7 +2942,7 @@
         <v>261</v>
       </c>
     </row>
-    <row ht="21" r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -2852,7 +2959,7 @@
         <v>262</v>
       </c>
     </row>
-    <row ht="21" r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -2869,7 +2976,7 @@
         <v>263</v>
       </c>
     </row>
-    <row ht="21" r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>86</v>
       </c>
@@ -2884,7 +2991,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>87</v>
       </c>
@@ -2898,7 +3005,7 @@
         <v>268</v>
       </c>
     </row>
-    <row ht="21" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -2913,7 +3020,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -2927,7 +3034,7 @@
         <v>270</v>
       </c>
     </row>
-    <row ht="21" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -2941,7 +3048,7 @@
         <v>270</v>
       </c>
     </row>
-    <row ht="21" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
@@ -2956,7 +3063,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>94</v>
       </c>
@@ -2970,7 +3077,7 @@
         <v>273</v>
       </c>
     </row>
-    <row ht="21" r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
@@ -2984,7 +3091,7 @@
         <v>301</v>
       </c>
     </row>
-    <row ht="21" r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>96</v>
       </c>
@@ -2999,7 +3106,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>154</v>
       </c>
@@ -3013,7 +3120,7 @@
         <v>281</v>
       </c>
     </row>
-    <row ht="21" r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>155</v>
       </c>
@@ -3027,7 +3134,7 @@
         <v>283</v>
       </c>
     </row>
-    <row ht="21" r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>162</v>
       </c>
@@ -3044,7 +3151,7 @@
         <v>285</v>
       </c>
     </row>
-    <row ht="21" r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>165</v>
       </c>
@@ -3059,7 +3166,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>166</v>
       </c>
@@ -3073,7 +3180,7 @@
         <v>287</v>
       </c>
     </row>
-    <row ht="21" r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>167</v>
       </c>
@@ -3087,7 +3194,7 @@
         <v>289</v>
       </c>
     </row>
-    <row ht="21" r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>182</v>
       </c>
@@ -3102,7 +3209,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>183</v>
       </c>
@@ -3116,7 +3223,7 @@
         <v>291</v>
       </c>
     </row>
-    <row ht="21" r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>184</v>
       </c>
@@ -3131,7 +3238,7 @@
         <v>264</v>
       </c>
     </row>
-    <row ht="21" r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>185</v>
       </c>
@@ -3147,11 +3254,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{71C2C0A5-75F0-C044-8439-AFDF571060AF}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71C2C0A5-75F0-C044-8439-AFDF571060AF}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$33</xm:f>
           </x14:formula1>
@@ -3164,8 +3271,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3EB00A-36E8-8846-87D3-B89735A262F1}">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3EB00A-36E8-8846-87D3-B89735A262F1}">
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -3173,16 +3280,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="10.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="14" width="42.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="14" width="28.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="14" width="50.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="14" width="39.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="14" width="99.6640625" collapsed="true"/>
-    <col min="7" max="16384" style="14" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="10.83203125" style="14" collapsed="1"/>
+    <col min="2" max="2" width="42" style="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50" style="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="99.6640625" style="14" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="10.83203125" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -3703,13 +3810,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5" xr:uid="{681CC5D2-C7F9-8C48-AD49-4568DD34C8C9}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{681CC5D2-C7F9-8C48-AD49-4568DD34C8C9}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{3E30CED1-26DB-6A45-8B25-994EB640CA91}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3E30CED1-26DB-6A45-8B25-994EB640CA91}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$33</xm:f>
           </x14:formula1>
@@ -3722,8 +3829,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB3DC7D-3A45-FC42-8060-5032618F8DB9}">
-  <dimension ref="A1:F48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB3DC7D-3A45-FC42-8060-5032618F8DB9}">
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
@@ -3731,12 +3838,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="42.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" width="42.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="21" r="1" s="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -3753,7 +3860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="2" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -3767,7 +3874,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="3" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -3784,7 +3891,7 @@
         <v>106</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="4" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -3801,7 +3908,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="5" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>74</v>
       </c>
@@ -3818,7 +3925,7 @@
         <v>108</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="6" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>75</v>
       </c>
@@ -3835,7 +3942,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="7" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -3850,7 +3957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="8" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
@@ -3864,7 +3971,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="9" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -3881,7 +3988,7 @@
         <v>123</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="10" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -3898,7 +4005,7 @@
         <v>111</v>
       </c>
     </row>
-    <row ht="21" r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>86</v>
       </c>
@@ -3913,7 +4020,7 @@
         <v>127</v>
       </c>
     </row>
-    <row ht="21" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>87</v>
       </c>
@@ -3928,7 +4035,7 @@
         <v>128</v>
       </c>
     </row>
-    <row ht="21" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -3943,7 +4050,7 @@
         <v>313</v>
       </c>
     </row>
-    <row ht="21" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -3958,7 +4065,7 @@
         <v>203</v>
       </c>
     </row>
-    <row ht="21" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -3973,7 +4080,7 @@
         <v>203</v>
       </c>
     </row>
-    <row ht="21" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
@@ -3988,7 +4095,7 @@
         <v>135</v>
       </c>
     </row>
-    <row ht="21" r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>94</v>
       </c>
@@ -4003,7 +4110,7 @@
         <v>135</v>
       </c>
     </row>
-    <row ht="21" r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
@@ -4020,7 +4127,7 @@
         <v>136</v>
       </c>
     </row>
-    <row ht="21" r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>96</v>
       </c>
@@ -4037,7 +4144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row ht="21" r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>97</v>
       </c>
@@ -4052,7 +4159,7 @@
         <v>138</v>
       </c>
     </row>
-    <row ht="21" r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>152</v>
       </c>
@@ -4067,7 +4174,7 @@
         <v>323</v>
       </c>
     </row>
-    <row ht="21" r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>153</v>
       </c>
@@ -4082,7 +4189,7 @@
         <v>204</v>
       </c>
     </row>
-    <row ht="21" r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>154</v>
       </c>
@@ -4097,7 +4204,7 @@
         <v>355</v>
       </c>
     </row>
-    <row ht="21" r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>155</v>
       </c>
@@ -4112,7 +4219,7 @@
         <v>352</v>
       </c>
     </row>
-    <row ht="21" r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>162</v>
       </c>
@@ -4127,7 +4234,7 @@
         <v>355</v>
       </c>
     </row>
-    <row ht="21" r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>165</v>
       </c>
@@ -4142,7 +4249,7 @@
         <v>325</v>
       </c>
     </row>
-    <row ht="21" r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>166</v>
       </c>
@@ -4157,7 +4264,7 @@
         <v>328</v>
       </c>
     </row>
-    <row ht="21" r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>167</v>
       </c>
@@ -4172,7 +4279,7 @@
         <v>328</v>
       </c>
     </row>
-    <row ht="21" r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>182</v>
       </c>
@@ -4187,7 +4294,7 @@
         <v>329</v>
       </c>
     </row>
-    <row ht="21" r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>183</v>
       </c>
@@ -4204,7 +4311,7 @@
         <v>330</v>
       </c>
     </row>
-    <row ht="21" r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>184</v>
       </c>
@@ -4219,7 +4326,7 @@
         <v>331</v>
       </c>
     </row>
-    <row ht="21" r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>185</v>
       </c>
@@ -4234,7 +4341,7 @@
         <v>141</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="33" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>186</v>
       </c>
@@ -4248,7 +4355,7 @@
         <v>205</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="34" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>187</v>
       </c>
@@ -4262,7 +4369,7 @@
         <v>206</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="35" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>188</v>
       </c>
@@ -4276,7 +4383,7 @@
         <v>206</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="36" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>189</v>
       </c>
@@ -4290,7 +4397,7 @@
         <v>207</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="37" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>341</v>
       </c>
@@ -4305,7 +4412,7 @@
         <v>207</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="38" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>342</v>
       </c>
@@ -4320,7 +4427,7 @@
         <v>175</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="39" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>343</v>
       </c>
@@ -4334,7 +4441,7 @@
         <v>175</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="40" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>344</v>
       </c>
@@ -4348,7 +4455,7 @@
         <v>335</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="41" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>345</v>
       </c>
@@ -4362,7 +4469,7 @@
         <v>208</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="42" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>346</v>
       </c>
@@ -4376,7 +4483,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="43" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>347</v>
       </c>
@@ -4390,7 +4497,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="44" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>348</v>
       </c>
@@ -4405,7 +4512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="45" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>349</v>
       </c>
@@ -4419,7 +4526,7 @@
         <v>180</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="46" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>350</v>
       </c>
@@ -4434,7 +4541,7 @@
         <v>181</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="47" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>351</v>
       </c>
@@ -4451,7 +4558,7 @@
         <v>230</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="48" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>354</v>
       </c>
@@ -4471,13 +4578,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5" xr:uid="{0B496968-09E8-A148-AF11-39A63A715C19}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{0B496968-09E8-A148-AF11-39A63A715C19}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{AFD83E70-D884-5F47-8AC6-350B03286A7E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFD83E70-D884-5F47-8AC6-350B03286A7E}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$29</xm:f>
           </x14:formula1>
@@ -4490,8 +4597,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CBE7D8-2A9B-4845-B1BD-72556917A96E}">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CBE7D8-2A9B-4845-B1BD-72556917A96E}">
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
@@ -4499,13 +4606,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="21" r="1" s="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -4522,7 +4629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="2" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -4536,7 +4643,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="3" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -4553,7 +4660,7 @@
         <v>106</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="4" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -4570,7 +4677,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="5" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>74</v>
       </c>
@@ -4587,7 +4694,7 @@
         <v>108</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="6" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>75</v>
       </c>
@@ -4604,7 +4711,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="7" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -4619,7 +4726,7 @@
         <v>85</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="8" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
@@ -4633,7 +4740,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="9" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -4650,7 +4757,7 @@
         <v>123</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="10" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -4667,7 +4774,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="11" s="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>86</v>
       </c>
@@ -4682,7 +4789,7 @@
         <v>143</v>
       </c>
     </row>
-    <row ht="21" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>87</v>
       </c>
@@ -4697,7 +4804,7 @@
         <v>144</v>
       </c>
     </row>
-    <row ht="21" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -4712,7 +4819,7 @@
         <v>209</v>
       </c>
     </row>
-    <row ht="21" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -4729,7 +4836,7 @@
         <v>149</v>
       </c>
     </row>
-    <row ht="21" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -4744,7 +4851,7 @@
         <v>210</v>
       </c>
     </row>
-    <row ht="21" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
@@ -4759,7 +4866,7 @@
         <v>211</v>
       </c>
     </row>
-    <row ht="21" r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>94</v>
       </c>
@@ -4774,7 +4881,7 @@
         <v>212</v>
       </c>
     </row>
-    <row ht="21" r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
@@ -4789,7 +4896,7 @@
         <v>202</v>
       </c>
     </row>
-    <row ht="21" r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>96</v>
       </c>
@@ -4804,7 +4911,7 @@
         <v>213</v>
       </c>
     </row>
-    <row ht="21" r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>97</v>
       </c>
@@ -4819,7 +4926,7 @@
         <v>214</v>
       </c>
     </row>
-    <row ht="21" r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>152</v>
       </c>
@@ -4834,7 +4941,7 @@
         <v>215</v>
       </c>
     </row>
-    <row ht="21" r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>153</v>
       </c>
@@ -4849,7 +4956,7 @@
         <v>150</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="23" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>154</v>
       </c>
@@ -4866,7 +4973,7 @@
         <v>231</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="24" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>155</v>
       </c>
@@ -4883,7 +4990,7 @@
         <v>150</v>
       </c>
     </row>
-    <row ht="21" r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>162</v>
       </c>
@@ -4897,7 +5004,7 @@
         <v>216</v>
       </c>
     </row>
-    <row ht="21" r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>165</v>
       </c>
@@ -4911,7 +5018,7 @@
         <v>217</v>
       </c>
     </row>
-    <row ht="21" r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>166</v>
       </c>
@@ -4925,7 +5032,7 @@
         <v>218</v>
       </c>
     </row>
-    <row ht="21" r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>167</v>
       </c>
@@ -4940,7 +5047,7 @@
         <v>198</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="29" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>182</v>
       </c>
@@ -4957,7 +5064,7 @@
         <v>232</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="30" s="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>183</v>
       </c>
@@ -4977,13 +5084,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5" xr:uid="{0FEFF791-E541-0545-B874-553631242F7E}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{0FEFF791-E541-0545-B874-553631242F7E}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{3822833E-B87C-1B43-9441-A6767BBD95ED}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3822833E-B87C-1B43-9441-A6767BBD95ED}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$29</xm:f>
           </x14:formula1>
@@ -4996,22 +5103,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C67F11-B389-8246-AC83-9E11E97E954F}">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C67F11-B389-8246-AC83-9E11E97E954F}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="21" r="1" s="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -5028,7 +5135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="2" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -5042,7 +5149,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="3" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -5059,7 +5166,7 @@
         <v>106</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="4" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -5076,7 +5183,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="5" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>74</v>
       </c>
@@ -5093,7 +5200,7 @@
         <v>108</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="6" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>75</v>
       </c>
@@ -5110,7 +5217,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="7" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -5125,7 +5232,7 @@
         <v>85</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="8" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
@@ -5139,7 +5246,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="9" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -5156,7 +5263,7 @@
         <v>123</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="10" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -5173,7 +5280,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="11" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>86</v>
       </c>
@@ -5188,7 +5295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="12" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>87</v>
       </c>
@@ -5202,7 +5309,7 @@
         <v>115</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="13" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -5217,7 +5324,7 @@
         <v>220</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="14" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -5234,7 +5341,7 @@
         <v>225</v>
       </c>
     </row>
-    <row ht="21" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -5251,7 +5358,7 @@
         <v>226</v>
       </c>
     </row>
-    <row ht="21" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
@@ -5268,7 +5375,7 @@
         <v>227</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="17" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>94</v>
       </c>
@@ -5283,7 +5390,7 @@
         <v>229</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="18" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
@@ -5298,7 +5405,7 @@
         <v>234</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="19" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>96</v>
       </c>
@@ -5315,7 +5422,7 @@
         <v>233</v>
       </c>
     </row>
-    <row customFormat="1" ht="21" r="20" s="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>97</v>
       </c>
@@ -5335,13 +5442,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5" xr:uid="{059FDB00-A838-7E4E-9118-810FC7583C3A}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{059FDB00-A838-7E4E-9118-810FC7583C3A}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{C14E7F1B-D4EF-6041-ABC6-F723D90AB0C8}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C14E7F1B-D4EF-6041-ABC6-F723D90AB0C8}">
           <x14:formula1>
             <xm:f>Keywords!$A$2:$A$29</xm:f>
           </x14:formula1>
@@ -5351,4 +5458,412 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE24B080-BF25-004D-AF94-C24D4FE48ED9}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>376</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>256</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="D19" t="s">
+        <v>382</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to TC005 and TC006
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Automation/Conclave UI/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akin.adebayo1/Documents/GitHub/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312C339C-F730-3447-AFA5-B2CE0774A412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE5C40D-6C8F-AE4B-A1C0-CA3AE82EB665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" tabRatio="752" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="11" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="TC004_OrgAdminCreateOrgContact" sheetId="25" r:id="rId8"/>
     <sheet name="TS005_OrgadminCreateRegistry" sheetId="26" r:id="rId9"/>
     <sheet name="TC004_ResetPassword" sheetId="19" r:id="rId10"/>
-    <sheet name="TC005-OrgAdminAddUser" sheetId="22" r:id="rId11"/>
+    <sheet name="TC005-OrgAdminAddDeleteUser" sheetId="22" r:id="rId11"/>
     <sheet name="TC006-OrgAdminEnable_DisableMFA" sheetId="23" r:id="rId12"/>
     <sheet name="TC007-OrgAdminDeleteOrgUSer" sheetId="24" r:id="rId13"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="490">
   <si>
     <t>TS_02</t>
   </si>
@@ -1221,9 +1221,6 @@
     <t>To enter random text [Format: Automation+random letters (5) ]</t>
   </si>
   <si>
-    <t>To verify that org Admin can add an Org user</t>
-  </si>
-  <si>
     <t>auto_snr_supplier@yopmail.com</t>
   </si>
   <si>
@@ -1248,9 +1245,6 @@
     <t>elm_addUsers</t>
   </si>
   <si>
-    <t>TS-13</t>
-  </si>
-  <si>
     <t>Wait for Add users page</t>
   </si>
   <si>
@@ -1326,9 +1320,6 @@
     <t>TC007-OrgAdminDeleteOrgUSer</t>
   </si>
   <si>
-    <t>Verify Org Admin can enable and also disable the additional security(MFA) for Org user</t>
-  </si>
-  <si>
     <t>To verify that org Admin can delete an Org user</t>
   </si>
   <si>
@@ -1606,6 +1597,36 @@
   </si>
   <si>
     <t>You have successfully removed additional registries from your organisation</t>
+  </si>
+  <si>
+    <t>To verify that org Admin can add and delete an Org user</t>
+  </si>
+  <si>
+    <t>Verify Org Admin can enable and disable the additional security(MFA) for Org user</t>
+  </si>
+  <si>
+    <t>Check if the Additional Security checkbox is checked</t>
+  </si>
+  <si>
+    <t>TS_44</t>
+  </si>
+  <si>
+    <t>TS_61</t>
+  </si>
+  <si>
+    <t>TS_62</t>
+  </si>
+  <si>
+    <t>TS_63</t>
+  </si>
+  <si>
+    <t>TS_64</t>
+  </si>
+  <si>
+    <t>TS_65</t>
+  </si>
+  <si>
+    <t>TS_66</t>
   </si>
 </sst>
 </file>
@@ -2435,26 +2456,26 @@
     </row>
     <row r="35" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -2823,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE24B080-BF25-004D-AF94-C24D4FE48ED9}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2915,7 +2936,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>108</v>
@@ -2932,7 +2953,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>109</v>
@@ -3006,13 +3027,13 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3020,14 +3041,14 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3035,27 +3056,27 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3063,52 +3084,52 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>36</v>
@@ -3117,71 +3138,71 @@
         <v>254</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D19" t="s">
         <v>375</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>376</v>
-      </c>
-      <c r="D19" t="s">
-        <v>377</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>121</v>
@@ -3191,12 +3212,12 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>104</v>
@@ -3209,7 +3230,7 @@
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>107</v>
@@ -3218,10 +3239,191 @@
         <v>40</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3231,10 +3433,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA5472-2B02-F049-85CB-88F3464A6385}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3323,7 +3525,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>108</v>
@@ -3340,7 +3542,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>109</v>
@@ -3414,13 +3616,13 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3428,14 +3630,14 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3443,16 +3645,13 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>378</v>
+        <v>11</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3460,13 +3659,13 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3474,25 +3673,27 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3500,13 +3701,16 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>369</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3514,13 +3718,16 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>254</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3528,14 +3735,16 @@
         <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>121</v>
+        <v>373</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="14"/>
+        <v>374</v>
+      </c>
+      <c r="D19" t="s">
+        <v>375</v>
+      </c>
       <c r="E19" s="14" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3543,27 +3752,27 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+        <v>11</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>107</v>
+        <v>379</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="14"/>
+        <v>11</v>
+      </c>
       <c r="E21" s="14" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3571,13 +3780,13 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3585,14 +3794,14 @@
         <v>154</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>359</v>
+        <v>121</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3600,30 +3809,29 @@
         <v>155</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>391</v>
+        <v>104</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>392</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>161</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>393</v>
+        <v>107</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>11</v>
+        <v>40</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3631,25 +3839,28 @@
         <v>164</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="14"/>
+      <c r="E26" s="14" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>165</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="D27" s="14"/>
       <c r="E27" s="14" t="s">
-        <v>397</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3657,13 +3868,13 @@
         <v>166</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3671,13 +3882,13 @@
         <v>181</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3692,7 +3903,7 @@
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3720,7 +3931,507 @@
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="D37" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="D49" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+    </row>
+    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="E61" s="14"/>
+    </row>
+    <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="14" t="s">
         <v>403</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+    </row>
+    <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3822,7 +4533,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>108</v>
@@ -3839,7 +4550,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>109</v>
@@ -3913,13 +4624,13 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3927,14 +4638,14 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3942,16 +4653,16 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3959,13 +4670,13 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3973,7 +4684,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>11</v>
@@ -3985,13 +4696,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3999,7 +4710,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C17" s="14"/>
       <c r="E17" s="14"/>
@@ -4009,13 +4720,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4023,13 +4734,13 @@
         <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4037,13 +4748,13 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4058,7 +4769,7 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4086,7 +4797,7 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -4098,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4197,10 +4908,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>354</v>
+        <v>480</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>239</v>
@@ -4211,10 +4922,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>389</v>
+        <v>481</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>239</v>
@@ -4225,10 +4936,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>239</v>
@@ -4239,10 +4950,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>240</v>
@@ -4253,10 +4964,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>240</v>
@@ -5573,7 +6284,7 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>17</v>
@@ -5588,7 +6299,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>12</v>
@@ -5649,7 +6360,7 @@
         <v>161</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>23</v>
@@ -5721,10 +6432,10 @@
         <v>182</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>119</v>
@@ -6212,7 +6923,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>12</v>
@@ -6227,7 +6938,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>19</v>
@@ -6242,7 +6953,7 @@
         <v>154</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>12</v>
@@ -6272,14 +6983,14 @@
         <v>161</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="20" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -6287,14 +6998,14 @@
         <v>164</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="20" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -6302,16 +7013,16 @@
         <v>165</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -6454,7 +7165,7 @@
         <v>338</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>17</v>
@@ -6469,7 +7180,7 @@
         <v>339</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>12</v>
@@ -6590,14 +7301,14 @@
         <v>347</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -6608,7 +7319,7 @@
         <v>172</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>328</v>
@@ -6619,7 +7330,7 @@
     </row>
     <row r="48" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>330</v>
@@ -6633,7 +7344,7 @@
     </row>
     <row r="49" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>173</v>
@@ -6648,7 +7359,7 @@
     </row>
     <row r="50" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>331</v>
@@ -6663,7 +7374,7 @@
     </row>
     <row r="51" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>199</v>
@@ -6677,7 +7388,7 @@
     </row>
     <row r="52" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>333</v>
@@ -6691,7 +7402,7 @@
     </row>
     <row r="53" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>175</v>
@@ -6705,7 +7416,7 @@
     </row>
     <row r="54" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>334</v>
@@ -6719,7 +7430,7 @@
     </row>
     <row r="55" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>176</v>
@@ -6733,7 +7444,7 @@
     </row>
     <row r="56" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B56" s="19" t="s">
         <v>335</v>
@@ -6748,7 +7459,7 @@
     </row>
     <row r="57" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>178</v>
@@ -6762,7 +7473,7 @@
     </row>
     <row r="58" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>336</v>
@@ -6777,7 +7488,7 @@
     </row>
     <row r="59" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>104</v>
@@ -6794,7 +7505,7 @@
     </row>
     <row r="60" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>107</v>
@@ -7521,7 +8232,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>19</v>
@@ -7535,7 +8246,7 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>18</v>
@@ -7550,7 +8261,7 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>11</v>
@@ -7564,7 +8275,7 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>17</v>
@@ -7578,7 +8289,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>18</v>
@@ -7593,13 +8304,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7607,13 +8318,13 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7666,7 +8377,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>17</v>
@@ -7681,7 +8392,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>12</v>
@@ -7743,7 +8454,7 @@
         <v>164</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>23</v>
@@ -7780,7 +8491,7 @@
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7803,7 +8514,7 @@
         <v>182</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>17</v>
@@ -7817,7 +8528,7 @@
         <v>183</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>18</v>
@@ -7832,14 +8543,14 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7847,10 +8558,10 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>119</v>
@@ -7960,7 +8671,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>200</v>
@@ -8189,7 +8900,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>19</v>
@@ -8203,7 +8914,7 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>18</v>
@@ -8218,7 +8929,7 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>11</v>
@@ -8232,7 +8943,7 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>17</v>
@@ -8246,7 +8957,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>18</v>
@@ -8261,13 +8972,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8275,13 +8986,13 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8289,13 +9000,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8341,7 +9052,7 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8369,7 +9080,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8384,7 +9095,7 @@
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8392,13 +9103,13 @@
         <v>161</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8412,10 +9123,10 @@
         <v>39</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8429,10 +9140,10 @@
         <v>40</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8440,14 +9151,14 @@
         <v>166</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8455,7 +9166,7 @@
         <v>181</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>17</v>
@@ -8469,7 +9180,7 @@
         <v>182</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>18</v>
@@ -8484,7 +9195,7 @@
         <v>183</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>23</v>
@@ -8498,16 +9209,16 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8515,16 +9226,16 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D33" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>473</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8532,13 +9243,13 @@
         <v>186</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8560,7 +9271,7 @@
         <v>188</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>11</v>
@@ -8574,13 +9285,13 @@
         <v>338</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8588,7 +9299,7 @@
         <v>339</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>18</v>
@@ -8609,10 +9320,10 @@
         <v>39</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8626,10 +9337,10 @@
         <v>40</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to TC006 and Manage User Object repo
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akin.adebayo1/Documents/GitHub/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AC95F4-2FE1-894C-AFA6-3FA1D5454D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8935E3F-F3CF-0F4A-9B62-A7E28A5CD564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="515">
   <si>
     <t>TS_02</t>
   </si>
@@ -1266,18 +1266,9 @@
     <t>Enter First name</t>
   </si>
   <si>
-    <t>Org</t>
-  </si>
-  <si>
-    <t>txt.fName</t>
-  </si>
-  <si>
     <t>Enter Last name</t>
   </si>
   <si>
-    <t>txt.lName</t>
-  </si>
-  <si>
     <t>Enter email Address</t>
   </si>
   <si>
@@ -1686,7 +1677,31 @@
     <t>You have successfully deleted the user account</t>
   </si>
   <si>
-    <t>deletion_expected_message</t>
+    <t>expected_deletion_message</t>
+  </si>
+  <si>
+    <t>You have successfully saved these changes</t>
+  </si>
+  <si>
+    <t>expected_sucessfully_saved_message</t>
+  </si>
+  <si>
+    <t>Scroll until Add aditional security checkbox is visible of the page</t>
+  </si>
+  <si>
+    <t>TS_67</t>
+  </si>
+  <si>
+    <t>TS_68</t>
+  </si>
+  <si>
+    <t>TS_69</t>
+  </si>
+  <si>
+    <t>TS_70</t>
+  </si>
+  <si>
+    <t>TS_71</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1819,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1851,7 +1866,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1911,11 +1926,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2541,26 +2555,26 @@
     </row>
     <row r="35" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -2931,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE24B080-BF25-004D-AF94-C24D4FE48ED9}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3203,8 +3217,8 @@
       <c r="C17" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>498</v>
+      <c r="E17" s="29" t="s">
+        <v>495</v>
       </c>
       <c r="F17" s="28"/>
     </row>
@@ -3213,13 +3227,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E18" s="32" t="s">
-        <v>499</v>
+      <c r="E18" s="29" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3227,16 +3241,16 @@
         <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D19" t="s">
-        <v>375</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>500</v>
+        <v>372</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3244,13 +3258,13 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3258,13 +3272,13 @@
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3272,13 +3286,13 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3293,7 +3307,7 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3303,14 +3317,14 @@
       <c r="B24" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="29" t="s">
         <v>39</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F24" s="14"/>
     </row>
@@ -3325,10 +3339,10 @@
         <v>40</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3336,13 +3350,13 @@
         <v>164</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3365,16 +3379,16 @@
         <v>166</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>500</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3382,13 +3396,13 @@
         <v>181</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3396,16 +3410,16 @@
         <v>182</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3413,13 +3427,13 @@
         <v>183</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -3427,13 +3441,13 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3441,13 +3455,13 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C33" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="C33" s="30" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3455,13 +3469,13 @@
         <v>186</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3469,13 +3483,13 @@
         <v>187</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3483,13 +3497,13 @@
         <v>188</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3504,7 +3518,7 @@
       </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3517,11 +3531,11 @@
       <c r="C38" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="33" t="s">
-        <v>508</v>
+      <c r="D38" s="30" t="s">
+        <v>505</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3535,24 +3549,25 @@
         <v>40</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA5472-2B02-F049-85CB-88F3464A6385}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3606,8 +3621,8 @@
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>105</v>
+      <c r="D3" s="14" t="s">
+        <v>300</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>106</v>
@@ -3703,8 +3718,8 @@
       <c r="C9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>112</v>
+      <c r="D9" s="14" t="s">
+        <v>302</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>123</v>
@@ -3819,14 +3834,11 @@
       <c r="B17" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>369</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>370</v>
+      <c r="C17" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3834,16 +3846,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>254</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>372</v>
+        <v>369</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3851,16 +3860,16 @@
         <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D19" t="s">
-        <v>375</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>376</v>
+        <v>372</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3868,13 +3877,13 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3882,13 +3891,13 @@
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3896,13 +3905,13 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3910,14 +3919,14 @@
         <v>154</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3927,11 +3936,15 @@
       <c r="B24" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+      <c r="D24" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
@@ -3943,11 +3956,11 @@
       <c r="C25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>383</v>
+      <c r="D25" s="19" t="s">
+        <v>498</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3955,13 +3968,13 @@
         <v>164</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -3979,75 +3992,81 @@
         <v>359</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="32" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="32" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="B29" s="31" t="s">
+        <v>378</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="32" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="C30" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="32" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-    </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D31" s="31" t="s">
+        <v>507</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="32" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="14" t="s">
-        <v>397</v>
+      <c r="D32" s="31" t="s">
+        <v>508</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4055,16 +4074,16 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>389</v>
+        <v>497</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4072,13 +4091,13 @@
         <v>186</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4086,25 +4105,33 @@
         <v>187</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>392</v>
+        <v>501</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="29"/>
+        <v>17</v>
+      </c>
+      <c r="D35" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>188</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>393</v>
+        <v>503</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>17</v>
+        <v>438</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>497</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>394</v>
+        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4112,16 +4139,13 @@
         <v>338</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>482</v>
+        <v>390</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="D37" s="30" t="b">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4129,27 +4153,31 @@
         <v>339</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>395</v>
+        <v>509</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>396</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="E38" s="14"/>
     </row>
     <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>340</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>381</v>
+        <v>479</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>11</v>
+        <v>412</v>
+      </c>
+      <c r="D39" s="13" t="b">
+        <v>0</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4157,14 +4185,13 @@
         <v>341</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>121</v>
+        <v>392</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="14"/>
+        <v>11</v>
+      </c>
       <c r="E40" s="14" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4172,27 +4199,30 @@
         <v>342</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>104</v>
+        <v>378</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
+        <v>11</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>343</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>507</v>
+      </c>
       <c r="E42" s="14" t="s">
-        <v>400</v>
+        <v>508</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4200,45 +4230,42 @@
         <v>344</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>398</v>
+        <v>104</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>399</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="E43" s="14"/>
     </row>
     <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>345</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>358</v>
+        <v>107</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="14"/>
+        <v>40</v>
+      </c>
       <c r="E44" s="14" t="s">
-        <v>359</v>
+        <v>397</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>376</v>
+        <v>11</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4246,13 +4273,14 @@
         <v>346</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>390</v>
+        <v>358</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D46" s="14"/>
       <c r="E46" s="14" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4260,299 +4288,403 @@
         <v>347</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="29"/>
+        <v>36</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>350</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>482</v>
+        <v>501</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="D49" s="28" t="b">
+        <v>17</v>
+      </c>
+      <c r="D49" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>396</v>
+        <v>497</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>395</v>
+        <v>503</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>11</v>
+        <v>438</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>497</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>396</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>121</v>
+        <v>509</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14" t="s">
-        <v>400</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>104</v>
+        <v>479</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
+        <v>412</v>
+      </c>
+      <c r="D53" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>107</v>
+        <v>392</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="14"/>
+        <v>11</v>
+      </c>
       <c r="E54" s="14" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>358</v>
+        <v>121</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="14"/>
+      <c r="D56" s="19" t="s">
+        <v>507</v>
+      </c>
       <c r="E56" s="14" t="s">
-        <v>359</v>
+        <v>508</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>388</v>
+        <v>104</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>389</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="E57" s="19"/>
     </row>
     <row r="58" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>390</v>
+        <v>107</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>11</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D58" s="14"/>
       <c r="E58" s="14" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="29"/>
+      <c r="E59" s="14" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>393</v>
+        <v>358</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="D60" s="14"/>
       <c r="E60" s="14" t="s">
-        <v>394</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C61" s="29"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="29"/>
+        <v>385</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>404</v>
+        <v>501</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="D63" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="E63" s="14" t="s">
-        <v>405</v>
+        <v>497</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>406</v>
+        <v>503</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>11</v>
+        <v>438</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>497</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>407</v>
+        <v>504</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>121</v>
+        <v>390</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D65" s="14"/>
       <c r="E65" s="14" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>104</v>
+        <v>398</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
+        <v>23</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B67" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C72" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="14" t="s">
-        <v>408</v>
+      <c r="D72" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4770,16 +4902,16 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4787,13 +4919,13 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4801,7 +4933,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>11</v>
@@ -4813,13 +4945,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4827,7 +4959,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C17" s="14"/>
       <c r="E17" s="14"/>
@@ -4837,13 +4969,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4851,13 +4983,13 @@
         <v>96</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4865,13 +4997,13 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4886,7 +5018,7 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -4914,7 +5046,7 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -5025,10 +5157,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>239</v>
@@ -5039,10 +5171,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>239</v>
@@ -5053,10 +5185,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>239</v>
@@ -5067,10 +5199,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>240</v>
@@ -5081,10 +5213,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>240</v>
@@ -6388,7 +6520,7 @@
         <v>96</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>11</v>
@@ -6417,7 +6549,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>17</v>
@@ -6432,7 +6564,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>12</v>
@@ -6493,7 +6625,7 @@
         <v>164</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>12</v>
@@ -6507,7 +6639,7 @@
         <v>165</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>23</v>
@@ -6579,10 +6711,10 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>119</v>
@@ -6718,13 +6850,13 @@
         <v>342</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6732,13 +6864,13 @@
         <v>343</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6746,7 +6878,7 @@
         <v>344</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>17</v>
@@ -7113,7 +7245,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>12</v>
@@ -7128,7 +7260,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>19</v>
@@ -7143,7 +7275,7 @@
         <v>154</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>12</v>
@@ -7173,14 +7305,14 @@
         <v>161</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7188,14 +7320,14 @@
         <v>164</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7203,16 +7335,16 @@
         <v>165</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7355,7 +7487,7 @@
         <v>338</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>17</v>
@@ -7370,7 +7502,7 @@
         <v>339</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>12</v>
@@ -7491,14 +7623,14 @@
         <v>347</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -7509,7 +7641,7 @@
         <v>172</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>328</v>
@@ -7520,7 +7652,7 @@
     </row>
     <row r="48" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>330</v>
@@ -7534,7 +7666,7 @@
     </row>
     <row r="49" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>173</v>
@@ -7549,7 +7681,7 @@
     </row>
     <row r="50" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>331</v>
@@ -7564,7 +7696,7 @@
     </row>
     <row r="51" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>199</v>
@@ -7578,7 +7710,7 @@
     </row>
     <row r="52" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>333</v>
@@ -7592,7 +7724,7 @@
     </row>
     <row r="53" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>175</v>
@@ -7606,7 +7738,7 @@
     </row>
     <row r="54" spans="1:5" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>334</v>
@@ -7620,7 +7752,7 @@
     </row>
     <row r="55" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>176</v>
@@ -7634,7 +7766,7 @@
     </row>
     <row r="56" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B56" s="19" t="s">
         <v>335</v>
@@ -7649,7 +7781,7 @@
     </row>
     <row r="57" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>178</v>
@@ -7663,7 +7795,7 @@
     </row>
     <row r="58" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>336</v>
@@ -7678,7 +7810,7 @@
     </row>
     <row r="59" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>104</v>
@@ -7695,7 +7827,7 @@
     </row>
     <row r="60" spans="1:5" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>107</v>
@@ -7712,40 +7844,40 @@
     </row>
     <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>17</v>
@@ -8467,7 +8599,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>19</v>
@@ -8481,7 +8613,7 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>18</v>
@@ -8496,7 +8628,7 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>11</v>
@@ -8510,7 +8642,7 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>17</v>
@@ -8524,7 +8656,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>18</v>
@@ -8539,13 +8671,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8553,13 +8685,13 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8597,7 +8729,7 @@
         <v>97</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>11</v>
@@ -8627,7 +8759,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>17</v>
@@ -8642,7 +8774,7 @@
         <v>154</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>12</v>
@@ -8704,7 +8836,7 @@
         <v>165</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>12</v>
@@ -8719,7 +8851,7 @@
         <v>166</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>23</v>
@@ -8756,7 +8888,7 @@
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8779,7 +8911,7 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>17</v>
@@ -8793,7 +8925,7 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>18</v>
@@ -8808,14 +8940,14 @@
         <v>186</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8823,10 +8955,10 @@
         <v>187</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>119</v>
@@ -8936,7 +9068,7 @@
         <v>39</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>200</v>
@@ -8964,29 +9096,29 @@
         <v>345</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8994,7 +9126,7 @@
         <v>346</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>17</v>
@@ -9210,7 +9342,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>19</v>
@@ -9224,7 +9356,7 @@
         <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>18</v>
@@ -9239,7 +9371,7 @@
         <v>88</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>11</v>
@@ -9253,7 +9385,7 @@
         <v>89</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>17</v>
@@ -9267,7 +9399,7 @@
         <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>18</v>
@@ -9282,13 +9414,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9296,13 +9428,13 @@
         <v>94</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9310,13 +9442,13 @@
         <v>95</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9362,7 +9494,7 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9390,7 +9522,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9405,7 +9537,7 @@
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9413,13 +9545,13 @@
         <v>161</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9433,10 +9565,10 @@
         <v>39</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9450,10 +9582,10 @@
         <v>40</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9461,14 +9593,14 @@
         <v>166</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9476,7 +9608,7 @@
         <v>181</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>17</v>
@@ -9490,7 +9622,7 @@
         <v>182</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>18</v>
@@ -9505,7 +9637,7 @@
         <v>183</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>23</v>
@@ -9519,16 +9651,16 @@
         <v>184</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9536,16 +9668,16 @@
         <v>185</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D33" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>470</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9553,13 +9685,13 @@
         <v>186</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9581,7 +9713,7 @@
         <v>188</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>11</v>
@@ -9595,13 +9727,13 @@
         <v>338</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9609,7 +9741,7 @@
         <v>339</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>18</v>
@@ -9630,10 +9762,10 @@
         <v>39</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9647,10 +9779,10 @@
         <v>40</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9658,14 +9790,14 @@
         <v>342</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9673,14 +9805,14 @@
         <v>343</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -9688,7 +9820,7 @@
         <v>344</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
updated scripts - group
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Automation/Conclave UI/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A2320E-7881-A040-A85E-1ABF9D9E3671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4121C3-2440-D940-8EE6-FEF57DAF835F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="11" r:id="rId1"/>
@@ -1677,9 +1677,6 @@
     <t>Wait for confirm user button clickable</t>
   </si>
   <si>
-    <t>Organisation Administrator</t>
-  </si>
-  <si>
     <t>Highlight search input</t>
   </si>
   <si>
@@ -1717,6 +1714,9 @@
   </si>
   <si>
     <t>To select a checkbox after replacing parameter. It will replace '#' in xpath with value in 'data' coulumn</t>
+  </si>
+  <si>
+    <t>Organisation User</t>
   </si>
 </sst>
 </file>
@@ -2587,18 +2587,18 @@
     </row>
     <row r="38" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>515</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>518</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -5100,7 +5100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -5138,7 +5138,7 @@
         <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5152,7 +5152,7 @@
         <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5166,7 +5166,7 @@
         <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5180,7 +5180,7 @@
         <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5188,7 +5188,7 @@
         <v>228</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>230</v>
@@ -5206,7 +5206,7 @@
         <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5220,7 +5220,7 @@
         <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5234,7 +5234,7 @@
         <v>230</v>
       </c>
       <c r="D9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5248,7 +5248,7 @@
         <v>230</v>
       </c>
       <c r="D10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -7937,8 +7937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CBE7D8-2A9B-4845-B1BD-72556917A96E}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8564,10 +8564,10 @@
         <v>334</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>476</v>
@@ -8595,7 +8595,7 @@
         <v>503</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>473</v>
@@ -8675,7 +8675,7 @@
         <v>36</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>506</v>
+        <v>519</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>476</v>
@@ -8700,7 +8700,7 @@
         <v>402</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>12</v>
@@ -8789,7 +8789,7 @@
         <v>426</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>19</v>
@@ -8818,13 +8818,13 @@
         <v>430</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -8832,7 +8832,7 @@
         <v>462</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>23</v>
@@ -8860,7 +8860,7 @@
         <v>464</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update Spreadsheet with TC007
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -5,27 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Automation/Conclave UI/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akin.adebayo1/Documents/GitHub/ccs-ppg-uiautomation-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C499439-F770-D94A-BB60-F67BAC7A46AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D5D165-B565-BD48-81E7-81BFF349C66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="752" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="11" r:id="rId1"/>
     <sheet name="TestCases" sheetId="4" r:id="rId2"/>
-    <sheet name="TC001_RegBuyerOrganisation" sheetId="20" r:id="rId3"/>
-    <sheet name="TC002_RegSupplierOrganisation" sheetId="21" r:id="rId4"/>
-    <sheet name="TC001_AddDeleteContact" sheetId="16" r:id="rId5"/>
-    <sheet name="TC002_AddDeleteSite" sheetId="17" r:id="rId6"/>
-    <sheet name="TC003_AddDeleteGroup" sheetId="18" r:id="rId7"/>
-    <sheet name="TC004_OrgAdminCreateOrgContact" sheetId="25" r:id="rId8"/>
-    <sheet name="TS005_OrgadminCreateRegistry" sheetId="26" r:id="rId9"/>
-    <sheet name="TC004_ResetPassword" sheetId="19" r:id="rId10"/>
-    <sheet name="TC005_OrgAdminAddUser" sheetId="22" r:id="rId11"/>
-    <sheet name="TC006-OrgAdminEnable_DisableMFA" sheetId="23" r:id="rId12"/>
-    <sheet name="TC007-OrgAdminDeleteOrgUSer" sheetId="24" r:id="rId13"/>
+    <sheet name="TC007-OrgAdminAddRolesToUser" sheetId="27" r:id="rId3"/>
+    <sheet name="TC001_RegBuyerOrganisation" sheetId="20" r:id="rId4"/>
+    <sheet name="TC002_RegSupplierOrganisation" sheetId="21" r:id="rId5"/>
+    <sheet name="TC001_AddDeleteContact" sheetId="16" r:id="rId6"/>
+    <sheet name="TC002_AddDeleteSite" sheetId="17" r:id="rId7"/>
+    <sheet name="TC003_AddDeleteGroup" sheetId="18" r:id="rId8"/>
+    <sheet name="TC004_OrgAdminCreateOrgContact" sheetId="25" r:id="rId9"/>
+    <sheet name="TS005_OrgadminCreateRegistry" sheetId="26" r:id="rId10"/>
+    <sheet name="TC004_ResetPassword" sheetId="19" r:id="rId11"/>
+    <sheet name="TC005_OrgAdminAddUser" sheetId="22" r:id="rId12"/>
+    <sheet name="TC006-OrgAdminEnable_DisableMFA" sheetId="23" r:id="rId13"/>
+    <sheet name="TC007-OrgAdminDeleteOrgUSer" sheetId="24" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="TC001_AddDeleteContact">TestCases!#REF!</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="556">
   <si>
     <t>TS_02</t>
   </si>
@@ -1717,6 +1718,114 @@
   </si>
   <si>
     <t>Organisation User</t>
+  </si>
+  <si>
+    <t>TC007-OrgAdminAddRolesToUser</t>
+  </si>
+  <si>
+    <t>To verify Org Admin can add role to user then delete it</t>
+  </si>
+  <si>
+    <t>Scroll to the until Roles section is visible</t>
+  </si>
+  <si>
+    <t>txt_roles</t>
+  </si>
+  <si>
+    <t>Check if the OrgAdmin-Dashboard Service checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_OrgAdmin_Dashboard</t>
+  </si>
+  <si>
+    <t>Click on the OrgAdmin-Dashboard service checkbox</t>
+  </si>
+  <si>
+    <t>Check if the OrgUser-Dashboard Service checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_OrgUser_DashboardService</t>
+  </si>
+  <si>
+    <t>Click on the OrgUser-Dashboard service checkbox</t>
+  </si>
+  <si>
+    <t>Check if the eSourcing As a Supplier checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_eSourcingServicesAsASupplier</t>
+  </si>
+  <si>
+    <t>Click on the eSourcing As a Supplier checkbox</t>
+  </si>
+  <si>
+    <t>Check if the Senior Supplier checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_SnrSupplier_BuyerSupplierInfo</t>
+  </si>
+  <si>
+    <t>Click on the Senior Supplier checkbox</t>
+  </si>
+  <si>
+    <t>Check if the Junior Supplier checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_JnrSupplier_BuyerSupplierInfo</t>
+  </si>
+  <si>
+    <t>Click on the Junior Supplier checkbox</t>
+  </si>
+  <si>
+    <t>Check if the Buyer Supplier Info checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_BuyerSupplierInfo_DashboardService</t>
+  </si>
+  <si>
+    <t>Click on the Buyer Supplier Info checkbox</t>
+  </si>
+  <si>
+    <t>Check if the eSourcing Service checkbox is ticked</t>
+  </si>
+  <si>
+    <t>chkbox_eSourcingServices_AddToDashboard</t>
+  </si>
+  <si>
+    <t>Click on the eSourcing Service checkbox</t>
+  </si>
+  <si>
+    <t>Scroll to the bottom of the page to see Save changes button</t>
+  </si>
+  <si>
+    <t>TS_68</t>
+  </si>
+  <si>
+    <t>TS_69</t>
+  </si>
+  <si>
+    <t>TS_70</t>
+  </si>
+  <si>
+    <t>TS_71</t>
+  </si>
+  <si>
+    <t>TS_72</t>
+  </si>
+  <si>
+    <t>TS_73</t>
+  </si>
+  <si>
+    <t>TS_74</t>
+  </si>
+  <si>
+    <t>TS_75</t>
+  </si>
+  <si>
+    <t>TS_76</t>
+  </si>
+  <si>
+    <t>TS_77</t>
   </si>
 </sst>
 </file>
@@ -2608,6 +2717,700 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74E2150-0FED-F24A-A5C1-F70208B8B334}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="61" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.1640625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{E41EC00C-38BA-D743-9E4C-AB0E79DAC3AC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0EF74-DB5C-A149-940C-5B858FA6A662}">
+          <x14:formula1>
+            <xm:f>Keywords!$A$2:$A$33</xm:f>
+          </x14:formula1>
+          <xm:sqref>C16 C19:C24 C28 C31 C35:C36</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C67F11-B389-8246-AC83-9E11E97E954F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -2965,7 +3768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE24B080-BF25-004D-AF94-C24D4FE48ED9}">
   <dimension ref="A1:F46"/>
   <sheetViews>
@@ -3682,7 +4485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA5472-2B02-F049-85CB-88F3464A6385}">
   <dimension ref="A1:E68"/>
   <sheetViews>
@@ -4730,7 +5533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A7A141-B8CB-A644-A76C-157ED6699F5E}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -5098,10 +5901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5251,6 +6054,14 @@
         <v>512</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" location="TC001_AddDeleteContact!A1" display="TC001_AddDeleteContact" xr:uid="{495083B3-A086-144F-A4CB-0341CFDA339F}"/>
@@ -5261,17 +6072,1220 @@
     <hyperlink ref="A8" location="'TC006-OrgAdminEnable_DisableMFA'!A1" display="TC006-OrgAdminEnable_DisableMFA" xr:uid="{E962CC8B-A86A-454B-AE90-36F79CBB608F}"/>
     <hyperlink ref="A9" location="TC004_OrgAdminCreateOrgContact!A1" display="TC004_OrgAdminCreateOrgContact" xr:uid="{CF672290-71BE-E546-832A-3507B606ED7B}"/>
     <hyperlink ref="A10" location="TS005_OrgadminCreateRegistry!A1" display="TS005_OrgadminCreateRegistry" xr:uid="{8BE668EC-DAE2-8C44-BF9D-5DC86D6F2DA9}"/>
+    <hyperlink ref="A11" location="'TC007-OrgAdminAddRolesToUser'!A1" display="TC007-OrgAdminAddRolesToUser" xr:uid="{173891FF-9F38-C644-A4B7-54172147C34F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7C6C46-92E1-6642-A85C-66A6A60ABA22}">
+  <dimension ref="A1:E78"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="14" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D40" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="14" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D42" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D44" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D46" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D48" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="14" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D50" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>545</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D62" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D63" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D64" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D65" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D66" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D67" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D68" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>549</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" display="mailto:auto_snr_supplier@yopmail.com" xr:uid="{B640E383-C8F9-1F45-A775-B1C366DCDFFE}"/>
+    <hyperlink ref="D21" r:id="rId2" display="http://yopmail.com/" xr:uid="{38F725EA-3EA1-944E-93A9-27B9167A6AB2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668AFD03-FEF2-3140-AF6D-190EC0470E79}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5777,7 +7791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3352E-5FAD-A043-B815-800E1B99D5C6}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -6245,7 +8259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3EB00A-36E8-8846-87D3-B89735A262F1}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -6934,7 +8948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB3DC7D-3A45-FC42-8060-5032618F8DB9}">
   <dimension ref="A1:E63"/>
   <sheetViews>
@@ -7933,11 +9947,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CBE7D8-2A9B-4845-B1BD-72556917A96E}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -8919,7 +10933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2898620-9CC7-5647-A027-6B2B9A954795}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -9660,698 +11674,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74E2150-0FED-F24A-A5C1-F70208B8B334}">
-  <dimension ref="A1:E43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="61" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.1640625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>436</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>440</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>444</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>450</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>448</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>453</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>454</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>455</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>457</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>456</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>470</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>471</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>472</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{E41EC00C-38BA-D743-9E4C-AB0E79DAC3AC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0EF74-DB5C-A149-940C-5B858FA6A662}">
-          <x14:formula1>
-            <xm:f>Keywords!$A$2:$A$33</xm:f>
-          </x14:formula1>
-          <xm:sqref>C16 C19:C24 C28 C31 C35:C36</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>